<commit_message>
Carga de archivos finales del TIC - Diego Moya
</commit_message>
<xml_diff>
--- a/DataProcessingFinal.xlsx
+++ b/DataProcessingFinal.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f138c2c5cef2cc1/DIEGO/EPN/TIC/TIC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3949" documentId="8_{2C99C8C5-4EC2-419D-A641-3712D057AB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B287E486-1309-4256-9770-DE40549F0203}"/>
+  <xr:revisionPtr revIDLastSave="3960" documentId="8_{2C99C8C5-4EC2-419D-A641-3712D057AB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B39AE549-7C75-4FEA-B403-B35F62E156D9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DB7AD4A9-AF05-4109-81CE-7D163F947196}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{DB7AD4A9-AF05-4109-81CE-7D163F947196}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla para Aprendizajes" sheetId="1" r:id="rId1"/>
     <sheet name="Tabla para Técnicas" sheetId="2" r:id="rId2"/>
     <sheet name="Tabla para Algortimos" sheetId="4" r:id="rId3"/>
     <sheet name="Tabla disponibilidad dataset" sheetId="6" r:id="rId4"/>
-    <sheet name="Tabla Articulos No Aplica" sheetId="5" r:id="rId5"/>
+    <sheet name="Tabla Nivel de Madurez" sheetId="7" r:id="rId5"/>
+    <sheet name="Tabla Articulos No Aplica" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tabla disponibilidad dataset'!$A$1:$D$173</definedName>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="796">
   <si>
     <t>AID</t>
   </si>
@@ -2783,12 +2784,33 @@
   <si>
     <t>Result partido-Pos jug(es)-Acc juego -Rend jug</t>
   </si>
+  <si>
+    <t xml:space="preserve"> Asociación</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Modelos Combinados/Otros</t>
+  </si>
+  <si>
+    <t>Política Basada en Gradiente</t>
+  </si>
+  <si>
+    <t>Reducción de Dimensionalidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Regresión</t>
+  </si>
+  <si>
+    <t>Suma de Técnicas</t>
+  </si>
+  <si>
+    <t>Clasificación2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2841,6 +2863,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -2892,7 +2933,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2928,12 +2969,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2952,12 +3002,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2983,12 +3027,35 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="76">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -3406,83 +3473,113 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{18106EEB-2C71-412D-84AC-82FBBBAE9017}" name="Table2" displayName="Table2" ref="A1:G173" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{18106EEB-2C71-412D-84AC-82FBBBAE9017}" name="Table2" displayName="Table2" ref="A1:G173" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
   <autoFilter ref="A1:G173" xr:uid="{18106EEB-2C71-412D-84AC-82FBBBAE9017}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3DAFD06C-117A-42EF-97A2-88D168B164E2}" name="AID" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{DC754382-2757-43FC-BAD9-3017734EB99A}" name="Aprendizaje Supervisado" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{62F61171-CC36-41AC-8EA1-B3813DB63F50}" name="Aprendizaje No Supervisado" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{8427BF46-EABB-4F6B-9F4F-44A4DA0B5EA0}" name="Aprendizaje Semi-Supervisado" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{328DC5F4-BFA5-474F-9B81-5A93BAC336F0}" name="Aprendizaje Reforzado" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{14481D17-3154-4E51-B51E-BD27233C902F}" name="Aprendizaje Profundo" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{22F3BE5F-7222-400C-BDC7-B325CED7EFE4}" name="Técnicas Integradas/Otras" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{3DAFD06C-117A-42EF-97A2-88D168B164E2}" name="AID" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{DC754382-2757-43FC-BAD9-3017734EB99A}" name="Aprendizaje Supervisado" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{62F61171-CC36-41AC-8EA1-B3813DB63F50}" name="Aprendizaje No Supervisado" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{8427BF46-EABB-4F6B-9F4F-44A4DA0B5EA0}" name="Aprendizaje Semi-Supervisado" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{328DC5F4-BFA5-474F-9B81-5A93BAC336F0}" name="Aprendizaje Reforzado" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{14481D17-3154-4E51-B51E-BD27233C902F}" name="Aprendizaje Profundo" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{22F3BE5F-7222-400C-BDC7-B325CED7EFE4}" name="Técnicas Integradas/Otras" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A791FB95-CDF8-44F7-9575-F562F955C95A}" name="Table24" displayName="Table24" ref="A1:Q173" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A791FB95-CDF8-44F7-9575-F562F955C95A}" name="Table24" displayName="Table24" ref="A1:Q173" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="A1:Q173" xr:uid="{18106EEB-2C71-412D-84AC-82FBBBAE9017}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{505DF980-E770-43BC-98EE-766F82C8D73E}" name="AID" totalsRowLabel="Total" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{63788FBB-8DB9-43AC-93C6-ADD0A5691CE1}" name="Clasificación" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{492C21D2-57AD-4C89-81C3-FAE01B555A9B}" name="Regresión" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{F3C27A53-722F-4755-ABB4-9F6FFEDA208A}" name="Agrupación" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{CDD96B2E-84DE-4B31-824C-0E1C93C135EA}" name="Reducción de dimensionalidad" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{994552DF-6007-4F5A-9C76-4882C18B65EB}" name="Asociación" dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="10" xr3:uid="{37B469C0-FB3D-4C9F-BA2E-EF5918E46DF6}" name="Propagación de etiquetas" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{44063038-27B0-49C0-A3C5-6D2028134BCF}" name="Co-entrenamiento" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{61937ACB-BA96-4C7F-B686-D8D1D4215E17}" name="Auto-entrenamiento" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="13" xr3:uid="{39716EFC-EBFB-43FA-9823-1042B6852043}" name="Política basada en Gradiente" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{B6531C27-598D-4D1B-BFCF-162D8F8D5BD5}" name="Q-Learning" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="11" xr3:uid="{DEFF9F26-199B-4D30-B42C-48EBE6EFA386}" name="Actor-Crítico" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="16" xr3:uid="{DB3AC674-6533-4628-A35D-2F295DF72765}" name="Redes neuronales artificiales" dataDxfId="37"/>
-    <tableColumn id="15" xr3:uid="{713E3333-ADA9-4436-A91F-1E124F6117C2}" name="Redes neuronales convolucionales" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{239A6F98-43AB-4A89-954F-D0D756B24821}" name="Redes neuronales recurrentes" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="17" xr3:uid="{4FCEA67D-CCB4-4649-98AD-62919422BAA9}" name="Autoencoders" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{711CA6B0-04A5-492F-84F2-433DEF2568E5}" name="Modelos Combinados/Otros" totalsRowFunction="count" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{505DF980-E770-43BC-98EE-766F82C8D73E}" name="AID" totalsRowLabel="Total" dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{63788FBB-8DB9-43AC-93C6-ADD0A5691CE1}" name="Clasificación" dataDxfId="62" totalsRowDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{492C21D2-57AD-4C89-81C3-FAE01B555A9B}" name="Regresión" dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{F3C27A53-722F-4755-ABB4-9F6FFEDA208A}" name="Agrupación" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{CDD96B2E-84DE-4B31-824C-0E1C93C135EA}" name="Reducción de dimensionalidad" dataDxfId="56" totalsRowDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{994552DF-6007-4F5A-9C76-4882C18B65EB}" name="Asociación" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{37B469C0-FB3D-4C9F-BA2E-EF5918E46DF6}" name="Propagación de etiquetas" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{44063038-27B0-49C0-A3C5-6D2028134BCF}" name="Co-entrenamiento" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{61937ACB-BA96-4C7F-B686-D8D1D4215E17}" name="Auto-entrenamiento" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="13" xr3:uid="{39716EFC-EBFB-43FA-9823-1042B6852043}" name="Política basada en Gradiente" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="12" xr3:uid="{B6531C27-598D-4D1B-BFCF-162D8F8D5BD5}" name="Q-Learning" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{DEFF9F26-199B-4D30-B42C-48EBE6EFA386}" name="Actor-Crítico" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="16" xr3:uid="{DB3AC674-6533-4628-A35D-2F295DF72765}" name="Redes neuronales artificiales" dataDxfId="40"/>
+    <tableColumn id="15" xr3:uid="{713E3333-ADA9-4436-A91F-1E124F6117C2}" name="Redes neuronales convolucionales" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="14" xr3:uid="{239A6F98-43AB-4A89-954F-D0D756B24821}" name="Redes neuronales recurrentes" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="17" xr3:uid="{4FCEA67D-CCB4-4649-98AD-62919422BAA9}" name="Autoencoders" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{711CA6B0-04A5-492F-84F2-433DEF2568E5}" name="Modelos Combinados/Otros" totalsRowFunction="count" dataDxfId="33" totalsRowDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F59C7DEA-B442-47E0-8AF1-E578078F84C5}" name="Table246" displayName="Table246" ref="A1:R173" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F59C7DEA-B442-47E0-8AF1-E578078F84C5}" name="Table246" displayName="Table246" ref="A1:R173" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:R173" xr:uid="{18106EEB-2C71-412D-84AC-82FBBBAE9017}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{98710081-3D9B-4215-A86E-A8C555258AB7}" name="AID" totalsRowLabel="Total" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{E80F5BE3-777A-4A07-9E9C-B2C67E2638C1}" name="Algoritmos de ML" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{89CDDBCE-399F-442A-88EE-B33F2C21190B}" name="Clasificación" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{135F5BBC-A24D-4271-AC8F-0CBA8534B2AD}" name="Regresión" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{8A54FF8F-35F8-4A48-A783-89D1F0DB0E07}" name="Agrupación" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{6154ABC8-5516-47B5-8B97-DF56B982EEF0}" name="Reducción de dimensionalidad" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{1A67D7AC-770C-444B-947B-519D498FE269}" name="Asociación" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{505FE67F-5D58-4415-A11B-916F3ABD4BEF}" name="Propagación de etiquetas" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{AFFF3BD9-0E25-4C25-AF73-58596A07BFB9}" name="Co-entrenamiento" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{2D84118B-DB91-4E72-8AC7-921B71585C2A}" name="Auto-entrenamiento" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{B7BE10F4-2390-4E90-941D-8AE76604B8E8}" name="Basada en Gradiente" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{204F8F8D-2F11-4355-92AA-4A4A9D1B3787}" name="Q-Learning" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{AC55EB18-51ED-4C30-937E-9AD30A79BE5A}" name="Actor-Crítico" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{E765104C-995A-4754-BC7B-485C7AB97B5F}" name="Redes neuronales artificiales" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{A4322F95-1B2D-4D86-92D3-74BC8F0493BD}" name="Redes neuronales convolucionales" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{BD48D9E7-D66E-42F2-8326-A767A8E95D23}" name="Redes neuronales recurrentes" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{3C5FC893-2B37-4722-8942-4D09EE688F11}" name="Autoencoders" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{9CE7EF42-F9AE-4C75-A700-71EACA97C549}" name="Modelos Combinados/Otros" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{98710081-3D9B-4215-A86E-A8C555258AB7}" name="AID" totalsRowLabel="Total" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{E80F5BE3-777A-4A07-9E9C-B2C67E2638C1}" name="Algoritmos de ML" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{89CDDBCE-399F-442A-88EE-B33F2C21190B}" name="Clasificación" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{135F5BBC-A24D-4271-AC8F-0CBA8534B2AD}" name="Regresión" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{8A54FF8F-35F8-4A48-A783-89D1F0DB0E07}" name="Agrupación" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{6154ABC8-5516-47B5-8B97-DF56B982EEF0}" name="Reducción de dimensionalidad" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{1A67D7AC-770C-444B-947B-519D498FE269}" name="Asociación" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{505FE67F-5D58-4415-A11B-916F3ABD4BEF}" name="Propagación de etiquetas" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{AFFF3BD9-0E25-4C25-AF73-58596A07BFB9}" name="Co-entrenamiento" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{2D84118B-DB91-4E72-8AC7-921B71585C2A}" name="Auto-entrenamiento" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{B7BE10F4-2390-4E90-941D-8AE76604B8E8}" name="Basada en Gradiente" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{204F8F8D-2F11-4355-92AA-4A4A9D1B3787}" name="Q-Learning" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{AC55EB18-51ED-4C30-937E-9AD30A79BE5A}" name="Actor-Crítico" dataDxfId="15"/>
+    <tableColumn id="14" xr3:uid="{E765104C-995A-4754-BC7B-485C7AB97B5F}" name="Redes neuronales artificiales" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{A4322F95-1B2D-4D86-92D3-74BC8F0493BD}" name="Redes neuronales convolucionales" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{BD48D9E7-D66E-42F2-8326-A767A8E95D23}" name="Redes neuronales recurrentes" dataDxfId="12"/>
+    <tableColumn id="17" xr3:uid="{3C5FC893-2B37-4722-8942-4D09EE688F11}" name="Autoencoders" dataDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{9CE7EF42-F9AE-4C75-A700-71EACA97C549}" name="Modelos Combinados/Otros" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{522A9726-1A06-4CF7-B438-290E0C03857F}" name="Table7" displayName="Table7" ref="A1:E38" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{84713A7B-3BBE-41BE-860F-5E6514A77FF1}" name="Table1" displayName="Table1" ref="A1:S174" totalsRowShown="0" headerRowBorderDxfId="2">
+  <autoFilter ref="A1:S174" xr:uid="{84713A7B-3BBE-41BE-860F-5E6514A77FF1}"/>
+  <tableColumns count="19">
+    <tableColumn id="19" xr3:uid="{0C20E877-5A3B-404C-BF29-942B9B0459D5}" name="AID"/>
+    <tableColumn id="21" xr3:uid="{71AE7C0B-D947-41A5-84BB-9260DE3E4639}" name="Año de publicación" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{5DE171B6-52B6-4D1E-B7E2-22A73F533651}" name=" Asociación"/>
+    <tableColumn id="2" xr3:uid="{3CAECBF2-8D0A-4EA1-ABB1-F1A8B5407682}" name="Agrupación"/>
+    <tableColumn id="3" xr3:uid="{0BDF7D34-464A-4CE3-AABA-A2A36EBEF330}" name="Actor-Crítico"/>
+    <tableColumn id="4" xr3:uid="{1CC72EF8-00D3-4C9F-8DCA-02394CE76BBD}" name="Auto-entrenamiento"/>
+    <tableColumn id="5" xr3:uid="{ED21D061-C813-454C-86CC-935C1E9794ED}" name="Autoencoders"/>
+    <tableColumn id="6" xr3:uid="{8D04644E-FC91-4B3E-A1A6-6A3F69F65743}" name="Clasificación2"/>
+    <tableColumn id="7" xr3:uid="{BD537D4B-3BD9-473D-A282-5F1F8D27EA6A}" name="Co-entrenamiento"/>
+    <tableColumn id="8" xr3:uid="{7F0DD705-2213-4680-B6E0-C056ED4F13B0}" name=" Modelos Combinados/Otros"/>
+    <tableColumn id="9" xr3:uid="{974341D4-CA9C-452F-9434-17178F933078}" name="Política Basada en Gradiente"/>
+    <tableColumn id="10" xr3:uid="{AEC7B48E-E874-4F57-AE04-D60C7DA7A2E8}" name="Propagación de etiquetas"/>
+    <tableColumn id="11" xr3:uid="{729829DD-AA17-45CC-9421-9FFFF1D492DA}" name="Q-Learning"/>
+    <tableColumn id="12" xr3:uid="{3F458537-5D6C-424F-85A6-650F983D7A39}" name="Redes neuronales artificiales"/>
+    <tableColumn id="13" xr3:uid="{E28A129D-8392-4476-999F-B2BD3F0961C3}" name="Redes neuronales convolucionales"/>
+    <tableColumn id="14" xr3:uid="{9A7B5FA8-049A-4239-94D7-765A9F578880}" name="Redes neuronales recurrentes"/>
+    <tableColumn id="15" xr3:uid="{4227378C-C70C-4016-85AE-46A448010D54}" name="Reducción de Dimensionalidad"/>
+    <tableColumn id="16" xr3:uid="{0FF73AD7-8CF8-45EF-B076-DDD5509742F2}" name=" Regresión"/>
+    <tableColumn id="18" xr3:uid="{5588D4DA-D36A-4DEE-8FD5-8855B24ECADB}" name="Suma de Técnicas" dataDxfId="0">
+      <calculatedColumnFormula>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{522A9726-1A06-4CF7-B438-290E0C03857F}" name="Table7" displayName="Table7" ref="A1:E38" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:E38" xr:uid="{522A9726-1A06-4CF7-B438-290E0C03857F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E519C815-7B92-4A2F-A3E2-2DF0F683DBD8}" name="AID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{42CC939C-17D9-4025-AB66-09ADD8E7A6DA}" name="Autor(es)" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{98C21274-043B-4E8E-93EE-AB9670339EA3}" name="Año de publicación" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{2F8F0008-3F78-48A4-9648-6105D70A0950}" name="Título" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{285CC646-FEF7-44B4-9D16-8A5BB01085AB}" name="Razón" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E519C815-7B92-4A2F-A3E2-2DF0F683DBD8}" name="AID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{42CC939C-17D9-4025-AB66-09ADD8E7A6DA}" name="Autor(es)" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{98C21274-043B-4E8E-93EE-AB9670339EA3}" name="Año de publicación" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{2F8F0008-3F78-48A4-9648-6105D70A0950}" name="Título" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{285CC646-FEF7-44B4-9D16-8A5BB01085AB}" name="Razón" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4162,7 +4259,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="13">
+      <c r="A25" s="11">
         <v>59</v>
       </c>
       <c r="B25" s="1"/>
@@ -4842,7 +4939,7 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="13">
+      <c r="A73" s="11">
         <v>201</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -4998,7 +5095,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A83" s="13">
+      <c r="A83" s="11">
         <v>228</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -5161,7 +5258,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="14">
+      <c r="A94" s="12">
         <v>251</v>
       </c>
       <c r="B94" s="1"/>
@@ -5379,7 +5476,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A110" s="15">
+      <c r="A110" s="13">
         <v>280</v>
       </c>
       <c r="B110" s="1"/>
@@ -5615,7 +5712,7 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A126" s="14">
+      <c r="A126" s="12">
         <v>316</v>
       </c>
       <c r="B126" s="1" t="s">
@@ -5632,7 +5729,7 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" s="16">
+      <c r="A127" s="14">
         <v>318</v>
       </c>
       <c r="B127" s="1" t="s">
@@ -6322,7 +6419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C641D74-7230-4C4D-AF31-A7672EEDE24C}">
   <dimension ref="A1:Q173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A155" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
@@ -10687,7 +10784,7 @@
   <dimension ref="A1:R173"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15577,8 +15674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B847EDB-47F7-40E7-8226-D332D9959443}">
   <dimension ref="A1:D173"/>
   <sheetViews>
-    <sheetView topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="D176" sqref="D176"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15589,16 +15686,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="19" t="s">
         <v>395</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="20" t="s">
         <v>626</v>
       </c>
     </row>
@@ -15612,7 +15709,7 @@
       <c r="C2" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>627</v>
       </c>
     </row>
@@ -15674,7 +15771,7 @@
       <c r="C7" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
@@ -15686,7 +15783,7 @@
       <c r="C8" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>628</v>
       </c>
     </row>
@@ -15700,7 +15797,7 @@
       <c r="C9" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>629</v>
       </c>
     </row>
@@ -15714,7 +15811,7 @@
       <c r="C10" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>630</v>
       </c>
     </row>
@@ -15740,7 +15837,7 @@
       <c r="C12" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
@@ -15800,7 +15897,7 @@
       <c r="C17" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>641</v>
       </c>
     </row>
@@ -15814,7 +15911,7 @@
       <c r="C18" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>642</v>
       </c>
     </row>
@@ -15828,7 +15925,7 @@
       <c r="C19" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="7" t="s">
         <v>631</v>
       </c>
     </row>
@@ -15854,7 +15951,7 @@
       <c r="C21" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>632</v>
       </c>
     </row>
@@ -15928,7 +16025,7 @@
       <c r="C27" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="7" t="s">
         <v>644</v>
       </c>
     </row>
@@ -15966,7 +16063,7 @@
       <c r="C30" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="8" t="s">
         <v>646</v>
       </c>
     </row>
@@ -15980,7 +16077,7 @@
       <c r="C31" s="5" t="s">
         <v>633</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="7" t="s">
         <v>647</v>
       </c>
     </row>
@@ -15997,7 +16094,7 @@
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" ht="288" x14ac:dyDescent="0.3">
-      <c r="A33" s="11">
+      <c r="A33" s="9">
         <v>83</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -16096,7 +16193,7 @@
       <c r="C41" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="7" t="s">
         <v>649</v>
       </c>
     </row>
@@ -16132,7 +16229,7 @@
       <c r="C44" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="8" t="s">
         <v>650</v>
       </c>
     </row>
@@ -16226,7 +16323,7 @@
       <c r="C52" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D52" s="8" t="s">
         <v>635</v>
       </c>
     </row>
@@ -16270,7 +16367,7 @@
       <c r="C56" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="8" t="s">
         <v>652</v>
       </c>
     </row>
@@ -16284,7 +16381,7 @@
       <c r="C57" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D57" s="9" t="s">
+      <c r="D57" s="7" t="s">
         <v>653</v>
       </c>
     </row>
@@ -16298,7 +16395,7 @@
       <c r="C58" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="D58" s="10" t="s">
+      <c r="D58" s="8" t="s">
         <v>654</v>
       </c>
     </row>
@@ -16322,7 +16419,7 @@
       <c r="C60" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="D60" s="8" t="s">
         <v>655</v>
       </c>
     </row>
@@ -16488,7 +16585,7 @@
       <c r="C75" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D75" s="7" t="s">
         <v>636</v>
       </c>
     </row>
@@ -16502,7 +16599,7 @@
       <c r="C76" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="D76" s="10" t="s">
+      <c r="D76" s="8" t="s">
         <v>637</v>
       </c>
     </row>
@@ -16550,7 +16647,7 @@
       <c r="C80" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="D80" s="10" t="s">
+      <c r="D80" s="8" t="s">
         <v>638</v>
       </c>
     </row>
@@ -16598,7 +16695,7 @@
       <c r="C84" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="D84" s="10"/>
+      <c r="D84" s="8"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
@@ -16632,7 +16729,7 @@
       <c r="C87" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="D87" s="9" t="s">
+      <c r="D87" s="7" t="s">
         <v>663</v>
       </c>
     </row>
@@ -16675,7 +16772,7 @@
       <c r="B91" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C91" s="9" t="s">
+      <c r="C91" s="7" t="s">
         <v>665</v>
       </c>
       <c r="D91" s="5"/>
@@ -16697,10 +16794,10 @@
       <c r="B93" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C93" s="9" t="s">
+      <c r="C93" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="D93" s="9" t="s">
+      <c r="D93" s="7" t="s">
         <v>346</v>
       </c>
     </row>
@@ -16734,7 +16831,7 @@
       <c r="C96" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="D96" s="10" t="s">
+      <c r="D96" s="8" t="s">
         <v>666</v>
       </c>
     </row>
@@ -16772,7 +16869,7 @@
       <c r="C99" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="D99" s="9" t="s">
+      <c r="D99" s="7" t="s">
         <v>646</v>
       </c>
     </row>
@@ -16783,10 +16880,10 @@
       <c r="B100" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C100" s="10" t="s">
+      <c r="C100" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="D100" s="10" t="s">
+      <c r="D100" s="8" t="s">
         <v>349</v>
       </c>
     </row>
@@ -16797,10 +16894,10 @@
       <c r="B101" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C101" s="9" t="s">
+      <c r="C101" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="D101" s="9" t="s">
+      <c r="D101" s="7" t="s">
         <v>350</v>
       </c>
     </row>
@@ -16814,7 +16911,7 @@
       <c r="C102" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="D102" s="10" t="s">
+      <c r="D102" s="8" t="s">
         <v>669</v>
       </c>
     </row>
@@ -16840,7 +16937,7 @@
       <c r="C104" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="D104" s="10" t="s">
+      <c r="D104" s="8" t="s">
         <v>670</v>
       </c>
     </row>
@@ -16851,7 +16948,7 @@
       <c r="B105" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="C105" s="9" t="s">
+      <c r="C105" s="7" t="s">
         <v>671</v>
       </c>
       <c r="D105" s="5"/>
@@ -16886,7 +16983,7 @@
       <c r="C108" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="D108" s="10" t="s">
+      <c r="D108" s="8" t="s">
         <v>646</v>
       </c>
     </row>
@@ -16910,7 +17007,7 @@
       <c r="C110" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="D110" s="10" t="s">
+      <c r="D110" s="8" t="s">
         <v>653</v>
       </c>
     </row>
@@ -16924,7 +17021,7 @@
       <c r="C111" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="D111" s="9" t="s">
+      <c r="D111" s="7" t="s">
         <v>653</v>
       </c>
     </row>
@@ -16948,7 +17045,7 @@
       <c r="C113" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="D113" s="10" t="s">
+      <c r="D113" s="8" t="s">
         <v>670</v>
       </c>
     </row>
@@ -16974,7 +17071,7 @@
       <c r="C115" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="D115" s="9" t="s">
+      <c r="D115" s="7" t="s">
         <v>673</v>
       </c>
     </row>
@@ -16985,10 +17082,10 @@
       <c r="B116" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C116" s="10" t="s">
+      <c r="C116" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="D116" s="10" t="s">
+      <c r="D116" s="8" t="s">
         <v>674</v>
       </c>
     </row>
@@ -17012,7 +17109,7 @@
       <c r="C118" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="D118" s="10" t="s">
+      <c r="D118" s="8" t="s">
         <v>675</v>
       </c>
     </row>
@@ -17026,7 +17123,7 @@
       <c r="C119" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="D119" s="9" t="s">
+      <c r="D119" s="7" t="s">
         <v>676</v>
       </c>
     </row>
@@ -17064,7 +17161,7 @@
       <c r="C122" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="D122" s="10" t="s">
+      <c r="D122" s="8" t="s">
         <v>349</v>
       </c>
     </row>
@@ -17089,10 +17186,10 @@
       <c r="B124" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C124" s="10" t="s">
+      <c r="C124" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="D124" s="10" t="s">
+      <c r="D124" s="8" t="s">
         <v>364</v>
       </c>
     </row>
@@ -17137,10 +17234,10 @@
       <c r="B128" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C128" s="10" t="s">
+      <c r="C128" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="D128" s="10" t="s">
+      <c r="D128" s="8" t="s">
         <v>681</v>
       </c>
     </row>
@@ -17164,7 +17261,7 @@
       <c r="C130" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="D130" s="10" t="s">
+      <c r="D130" s="8" t="s">
         <v>682</v>
       </c>
     </row>
@@ -17175,7 +17272,7 @@
       <c r="B131" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="C131" s="9"/>
+      <c r="C131" s="7"/>
       <c r="D131" s="5"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -17215,10 +17312,10 @@
       <c r="B135" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C135" s="9" t="s">
+      <c r="C135" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="D135" s="9" t="s">
+      <c r="D135" s="7" t="s">
         <v>368</v>
       </c>
     </row>
@@ -17229,10 +17326,10 @@
       <c r="B136" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C136" s="10" t="s">
+      <c r="C136" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="D136" s="10" t="s">
+      <c r="D136" s="8" t="s">
         <v>369</v>
       </c>
     </row>
@@ -17246,7 +17343,7 @@
       <c r="C137" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="D137" s="9" t="s">
+      <c r="D137" s="7" t="s">
         <v>349</v>
       </c>
     </row>
@@ -17260,7 +17357,7 @@
       <c r="C138" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="D138" s="10" t="s">
+      <c r="D138" s="8" t="s">
         <v>683</v>
       </c>
     </row>
@@ -17274,7 +17371,7 @@
       <c r="C139" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="D139" s="9" t="s">
+      <c r="D139" s="7" t="s">
         <v>684</v>
       </c>
     </row>
@@ -17340,7 +17437,7 @@
       <c r="C145" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="D145" s="9" t="s">
+      <c r="D145" s="7" t="s">
         <v>686</v>
       </c>
     </row>
@@ -17398,7 +17495,7 @@
       <c r="C150" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="D150" s="10" t="s">
+      <c r="D150" s="8" t="s">
         <v>349</v>
       </c>
     </row>
@@ -17422,7 +17519,7 @@
       <c r="C152" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="D152" s="10" t="s">
+      <c r="D152" s="8" t="s">
         <v>634</v>
       </c>
     </row>
@@ -17436,7 +17533,7 @@
       <c r="C153" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D153" s="9" t="s">
+      <c r="D153" s="7" t="s">
         <v>634</v>
       </c>
     </row>
@@ -17480,7 +17577,7 @@
       <c r="C157" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="D157" s="9" t="s">
+      <c r="D157" s="7" t="s">
         <v>634</v>
       </c>
     </row>
@@ -17494,7 +17591,7 @@
       <c r="C158" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D158" s="10" t="s">
+      <c r="D158" s="8" t="s">
         <v>688</v>
       </c>
     </row>
@@ -17508,7 +17605,7 @@
       <c r="C159" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="D159" s="9" t="s">
+      <c r="D159" s="7" t="s">
         <v>689</v>
       </c>
     </row>
@@ -17522,7 +17619,7 @@
       <c r="C160" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="D160" s="10" t="s">
+      <c r="D160" s="8" t="s">
         <v>690</v>
       </c>
     </row>
@@ -17536,7 +17633,7 @@
       <c r="C161" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="D161" s="9" t="s">
+      <c r="D161" s="7" t="s">
         <v>349</v>
       </c>
     </row>
@@ -17550,7 +17647,7 @@
       <c r="C162" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D162" s="10" t="s">
+      <c r="D162" s="8" t="s">
         <v>393</v>
       </c>
     </row>
@@ -17564,7 +17661,7 @@
       <c r="C163" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="D163" s="9" t="s">
+      <c r="D163" s="7" t="s">
         <v>691</v>
       </c>
     </row>
@@ -17578,7 +17675,7 @@
       <c r="C164" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="D164" s="10" t="s">
+      <c r="D164" s="8" t="s">
         <v>692</v>
       </c>
     </row>
@@ -17604,7 +17701,7 @@
       <c r="C166" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="D166" s="10" t="s">
+      <c r="D166" s="8" t="s">
         <v>693</v>
       </c>
     </row>
@@ -17615,10 +17712,10 @@
       <c r="B167" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C167" s="9" t="s">
+      <c r="C167" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="D167" s="9" t="s">
+      <c r="D167" s="7" t="s">
         <v>393</v>
       </c>
     </row>
@@ -17632,7 +17729,7 @@
       <c r="C168" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="D168" s="10" t="s">
+      <c r="D168" s="8" t="s">
         <v>389</v>
       </c>
     </row>
@@ -17646,7 +17743,7 @@
       <c r="C169" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="D169" s="9" t="s">
+      <c r="D169" s="7" t="s">
         <v>390</v>
       </c>
     </row>
@@ -17657,10 +17754,10 @@
       <c r="B170" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C170" s="10" t="s">
+      <c r="C170" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="D170" s="10" t="s">
+      <c r="D170" s="8" t="s">
         <v>694</v>
       </c>
     </row>
@@ -17674,7 +17771,7 @@
       <c r="C171" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="D171" s="9" t="s">
+      <c r="D171" s="7" t="s">
         <v>670</v>
       </c>
     </row>
@@ -17685,10 +17782,10 @@
       <c r="B172" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="C172" s="10" t="s">
+      <c r="C172" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="D172" s="10" t="s">
+      <c r="D172" s="8" t="s">
         <v>393</v>
       </c>
     </row>
@@ -17702,7 +17799,7 @@
       <c r="C173" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="D173" s="12" t="s">
+      <c r="D173" s="10" t="s">
         <v>695</v>
       </c>
     </row>
@@ -17794,6 +17891,3209 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2349CD-1EF4-4DF8-8C76-114F9E823895}">
+  <dimension ref="A1:S174"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="3" max="19" width="19.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>789</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>795</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>790</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>791</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>792</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>793</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="16">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2024</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2024</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2024</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2023</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>48</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2023</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>57</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2024</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>58</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2023</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>64</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2023</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="16">
+        <v>66</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2023</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
+        <v>67</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" s="16">
+        <v>69</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" s="16">
+        <v>74</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" s="16">
+        <v>77</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32" s="16">
+        <v>80</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A33" s="16">
+        <v>83</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A34" s="16">
+        <v>86</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A35" s="16">
+        <v>87</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="S35">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A36" s="16">
+        <v>91</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A37" s="16">
+        <v>95</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2023</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="R37">
+        <v>1</v>
+      </c>
+      <c r="S37">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38" s="16">
+        <v>99</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2024</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="S38">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A39" s="16">
+        <v>103</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="S39">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A40" s="16">
+        <v>104</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="R40">
+        <v>1</v>
+      </c>
+      <c r="S40">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A41" s="16">
+        <v>109</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" s="16">
+        <v>110</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="S42">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A43" s="16">
+        <v>111</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="S43">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A44" s="16">
+        <v>112</v>
+      </c>
+      <c r="B44" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="S44">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="16">
+        <v>113</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="Q45">
+        <v>1</v>
+      </c>
+      <c r="S45">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" s="16">
+        <v>114</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="S46">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A47" s="16">
+        <v>120</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="R47">
+        <v>1</v>
+      </c>
+      <c r="S47">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" s="16">
+        <v>121</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="S48">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="16">
+        <v>124</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="R49">
+        <v>1</v>
+      </c>
+      <c r="S49">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A50" s="16">
+        <v>126</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="S50">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A51" s="16">
+        <v>127</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="S51">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A52" s="16">
+        <v>131</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="S52">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="16">
+        <v>132</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="S53">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" s="16">
+        <v>135</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2022</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
+      <c r="S54">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A55" s="16">
+        <v>151</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="S55">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A56" s="16">
+        <v>152</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="S56">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A57" s="16">
+        <v>155</v>
+      </c>
+      <c r="B57" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="S57">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A58" s="16">
+        <v>159</v>
+      </c>
+      <c r="B58" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="S58">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A59" s="16">
+        <v>160</v>
+      </c>
+      <c r="B59" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="S59">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A60" s="16">
+        <v>162</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <v>1</v>
+      </c>
+      <c r="O60">
+        <v>1</v>
+      </c>
+      <c r="P60">
+        <v>1</v>
+      </c>
+      <c r="S60">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A61" s="16">
+        <v>174</v>
+      </c>
+      <c r="B61" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="S61">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A62" s="16">
+        <v>176</v>
+      </c>
+      <c r="B62" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="S62">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A63" s="16">
+        <v>179</v>
+      </c>
+      <c r="B63" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="S63">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A64" s="16">
+        <v>182</v>
+      </c>
+      <c r="B64" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="S64">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A65" s="16">
+        <v>183</v>
+      </c>
+      <c r="B65" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="R65">
+        <v>1</v>
+      </c>
+      <c r="S65">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A66" s="16">
+        <v>185</v>
+      </c>
+      <c r="B66" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="S66">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A67" s="16">
+        <v>186</v>
+      </c>
+      <c r="B67" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="N67">
+        <v>1</v>
+      </c>
+      <c r="S67">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A68" s="16">
+        <v>188</v>
+      </c>
+      <c r="B68" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="S68">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A69" s="16">
+        <v>190</v>
+      </c>
+      <c r="B69" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="S69">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A70" s="16">
+        <v>192</v>
+      </c>
+      <c r="B70" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="S70">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A71" s="16">
+        <v>194</v>
+      </c>
+      <c r="B71" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="S71">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A72" s="16">
+        <v>198</v>
+      </c>
+      <c r="B72" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="O72">
+        <v>1</v>
+      </c>
+      <c r="P72">
+        <v>1</v>
+      </c>
+      <c r="Q72">
+        <v>1</v>
+      </c>
+      <c r="R72">
+        <v>1</v>
+      </c>
+      <c r="S72">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A73" s="16">
+        <v>201</v>
+      </c>
+      <c r="B73" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="N73">
+        <v>1</v>
+      </c>
+      <c r="R73">
+        <v>1</v>
+      </c>
+      <c r="S73">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A74" s="16">
+        <v>204</v>
+      </c>
+      <c r="B74" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="R74">
+        <v>1</v>
+      </c>
+      <c r="S74">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A75" s="16">
+        <v>206</v>
+      </c>
+      <c r="B75" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="S75">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A76" s="16">
+        <v>207</v>
+      </c>
+      <c r="B76" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+      <c r="S76">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A77" s="16">
+        <v>208</v>
+      </c>
+      <c r="B77" s="1">
+        <v>2021</v>
+      </c>
+      <c r="N77">
+        <v>1</v>
+      </c>
+      <c r="S77">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A78" s="16">
+        <v>210</v>
+      </c>
+      <c r="B78" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="N78">
+        <v>1</v>
+      </c>
+      <c r="S78">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A79" s="16">
+        <v>212</v>
+      </c>
+      <c r="B79" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="N79">
+        <v>1</v>
+      </c>
+      <c r="S79">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A80" s="16">
+        <v>213</v>
+      </c>
+      <c r="B80" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="N80">
+        <v>1</v>
+      </c>
+      <c r="S80">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A81" s="16">
+        <v>220</v>
+      </c>
+      <c r="B81" s="1">
+        <v>2022</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="N81">
+        <v>1</v>
+      </c>
+      <c r="O81">
+        <v>1</v>
+      </c>
+      <c r="S81">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A82" s="16">
+        <v>223</v>
+      </c>
+      <c r="B82" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+      <c r="S82">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A83" s="16">
+        <v>228</v>
+      </c>
+      <c r="B83" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="S83">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A84" s="16">
+        <v>230</v>
+      </c>
+      <c r="B84" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="N84">
+        <v>1</v>
+      </c>
+      <c r="S84">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A85" s="16">
+        <v>231</v>
+      </c>
+      <c r="B85" s="1">
+        <v>2022</v>
+      </c>
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="S85">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A86" s="16">
+        <v>232</v>
+      </c>
+      <c r="B86" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="N86">
+        <v>1</v>
+      </c>
+      <c r="P86">
+        <v>1</v>
+      </c>
+      <c r="S86">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A87" s="16">
+        <v>236</v>
+      </c>
+      <c r="B87" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+      <c r="S87">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A88" s="16">
+        <v>238</v>
+      </c>
+      <c r="B88" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>1</v>
+      </c>
+      <c r="O88">
+        <v>1</v>
+      </c>
+      <c r="S88">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A89" s="16">
+        <v>241</v>
+      </c>
+      <c r="B89" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <v>1</v>
+      </c>
+      <c r="S89">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A90" s="16">
+        <v>242</v>
+      </c>
+      <c r="B90" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="S90">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A91" s="16">
+        <v>245</v>
+      </c>
+      <c r="B91" s="1">
+        <v>2021</v>
+      </c>
+      <c r="O91">
+        <v>1</v>
+      </c>
+      <c r="P91">
+        <v>1</v>
+      </c>
+      <c r="S91">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A92" s="16">
+        <v>246</v>
+      </c>
+      <c r="B92" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="R92">
+        <v>1</v>
+      </c>
+      <c r="S92">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A93" s="16">
+        <v>249</v>
+      </c>
+      <c r="B93" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="J93">
+        <v>1</v>
+      </c>
+      <c r="N93">
+        <v>1</v>
+      </c>
+      <c r="S93">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A94" s="16">
+        <v>251</v>
+      </c>
+      <c r="B94" s="1">
+        <v>2021</v>
+      </c>
+      <c r="N94">
+        <v>1</v>
+      </c>
+      <c r="S94">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A95" s="16">
+        <v>252</v>
+      </c>
+      <c r="B95" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="R95">
+        <v>1</v>
+      </c>
+      <c r="S95">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A96" s="16">
+        <v>255</v>
+      </c>
+      <c r="B96" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="S96">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A97" s="16">
+        <v>256</v>
+      </c>
+      <c r="B97" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="N97">
+        <v>1</v>
+      </c>
+      <c r="S97">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A98" s="16">
+        <v>259</v>
+      </c>
+      <c r="B98" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="S98">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A99" s="16">
+        <v>260</v>
+      </c>
+      <c r="B99" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="J99">
+        <v>1</v>
+      </c>
+      <c r="R99">
+        <v>1</v>
+      </c>
+      <c r="S99">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A100" s="16">
+        <v>261</v>
+      </c>
+      <c r="B100" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="S100">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A101" s="16">
+        <v>264</v>
+      </c>
+      <c r="B101" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H101">
+        <v>1</v>
+      </c>
+      <c r="R101">
+        <v>1</v>
+      </c>
+      <c r="S101">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A102" s="16">
+        <v>265</v>
+      </c>
+      <c r="B102" s="1">
+        <v>2022</v>
+      </c>
+      <c r="N102">
+        <v>1</v>
+      </c>
+      <c r="S102">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A103" s="16">
+        <v>266</v>
+      </c>
+      <c r="B103" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+      <c r="Q103">
+        <v>1</v>
+      </c>
+      <c r="S103">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A104" s="16">
+        <v>267</v>
+      </c>
+      <c r="B104" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+      <c r="J104">
+        <v>1</v>
+      </c>
+      <c r="S104">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A105" s="16">
+        <v>268</v>
+      </c>
+      <c r="B105" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J105">
+        <v>1</v>
+      </c>
+      <c r="S105">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A106" s="16">
+        <v>271</v>
+      </c>
+      <c r="B106" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H106">
+        <v>1</v>
+      </c>
+      <c r="S106">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A107" s="16">
+        <v>272</v>
+      </c>
+      <c r="B107" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="J107">
+        <v>1</v>
+      </c>
+      <c r="Q107">
+        <v>1</v>
+      </c>
+      <c r="S107">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A108" s="16">
+        <v>273</v>
+      </c>
+      <c r="B108" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H108">
+        <v>1</v>
+      </c>
+      <c r="J108">
+        <v>1</v>
+      </c>
+      <c r="S108">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A109" s="16">
+        <v>275</v>
+      </c>
+      <c r="B109" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J109">
+        <v>1</v>
+      </c>
+      <c r="S109">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A110" s="16">
+        <v>280</v>
+      </c>
+      <c r="B110" s="1">
+        <v>2021</v>
+      </c>
+      <c r="N110">
+        <v>1</v>
+      </c>
+      <c r="S110">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A111" s="16">
+        <v>281</v>
+      </c>
+      <c r="B111" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J111">
+        <v>1</v>
+      </c>
+      <c r="S111">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A112" s="16">
+        <v>282</v>
+      </c>
+      <c r="B112" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H112">
+        <v>1</v>
+      </c>
+      <c r="J112">
+        <v>1</v>
+      </c>
+      <c r="N112">
+        <v>1</v>
+      </c>
+      <c r="R112">
+        <v>1</v>
+      </c>
+      <c r="S112">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A113" s="16">
+        <v>283</v>
+      </c>
+      <c r="B113" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H113">
+        <v>1</v>
+      </c>
+      <c r="J113">
+        <v>1</v>
+      </c>
+      <c r="S113">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A114" s="16">
+        <v>288</v>
+      </c>
+      <c r="B114" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J114">
+        <v>1</v>
+      </c>
+      <c r="S114">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A115" s="16">
+        <v>292</v>
+      </c>
+      <c r="B115" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J115">
+        <v>1</v>
+      </c>
+      <c r="R115">
+        <v>1</v>
+      </c>
+      <c r="S115">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A116" s="16">
+        <v>293</v>
+      </c>
+      <c r="B116" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="K116">
+        <v>1</v>
+      </c>
+      <c r="M116">
+        <v>1</v>
+      </c>
+      <c r="N116">
+        <v>1</v>
+      </c>
+      <c r="S116">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A117" s="16">
+        <v>298</v>
+      </c>
+      <c r="B117" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J117">
+        <v>1</v>
+      </c>
+      <c r="S117">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A118" s="16">
+        <v>299</v>
+      </c>
+      <c r="B118" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J118">
+        <v>1</v>
+      </c>
+      <c r="S118">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A119" s="16">
+        <v>301</v>
+      </c>
+      <c r="B119" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="H119">
+        <v>1</v>
+      </c>
+      <c r="N119">
+        <v>1</v>
+      </c>
+      <c r="S119">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A120" s="16">
+        <v>302</v>
+      </c>
+      <c r="B120" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H120">
+        <v>1</v>
+      </c>
+      <c r="N120">
+        <v>1</v>
+      </c>
+      <c r="S120">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A121" s="16">
+        <v>310</v>
+      </c>
+      <c r="B121" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H121">
+        <v>1</v>
+      </c>
+      <c r="N121">
+        <v>1</v>
+      </c>
+      <c r="Q121">
+        <v>1</v>
+      </c>
+      <c r="S121">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A122" s="16">
+        <v>312</v>
+      </c>
+      <c r="B122" s="1">
+        <v>2020</v>
+      </c>
+      <c r="P122">
+        <v>1</v>
+      </c>
+      <c r="S122">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A123" s="16">
+        <v>313</v>
+      </c>
+      <c r="B123" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H123">
+        <v>1</v>
+      </c>
+      <c r="J123">
+        <v>1</v>
+      </c>
+      <c r="Q123">
+        <v>1</v>
+      </c>
+      <c r="S123">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A124" s="16">
+        <v>314</v>
+      </c>
+      <c r="B124" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H124">
+        <v>1</v>
+      </c>
+      <c r="J124">
+        <v>1</v>
+      </c>
+      <c r="S124">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A125" s="16">
+        <v>315</v>
+      </c>
+      <c r="B125" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H125">
+        <v>1</v>
+      </c>
+      <c r="J125">
+        <v>1</v>
+      </c>
+      <c r="R125">
+        <v>1</v>
+      </c>
+      <c r="S125">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A126" s="16">
+        <v>316</v>
+      </c>
+      <c r="B126" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H126">
+        <v>1</v>
+      </c>
+      <c r="J126">
+        <v>1</v>
+      </c>
+      <c r="N126">
+        <v>1</v>
+      </c>
+      <c r="R126">
+        <v>1</v>
+      </c>
+      <c r="S126">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A127" s="16">
+        <v>318</v>
+      </c>
+      <c r="B127" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H127">
+        <v>1</v>
+      </c>
+      <c r="J127">
+        <v>1</v>
+      </c>
+      <c r="Q127">
+        <v>1</v>
+      </c>
+      <c r="R127">
+        <v>1</v>
+      </c>
+      <c r="S127">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A128" s="16">
+        <v>322</v>
+      </c>
+      <c r="B128" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H128">
+        <v>1</v>
+      </c>
+      <c r="J128">
+        <v>1</v>
+      </c>
+      <c r="S128">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A129" s="16">
+        <v>324</v>
+      </c>
+      <c r="B129" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H129">
+        <v>1</v>
+      </c>
+      <c r="N129">
+        <v>1</v>
+      </c>
+      <c r="S129">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A130" s="16">
+        <v>325</v>
+      </c>
+      <c r="B130" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H130">
+        <v>1</v>
+      </c>
+      <c r="N130">
+        <v>1</v>
+      </c>
+      <c r="S130">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A131" s="16">
+        <v>329</v>
+      </c>
+      <c r="B131" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H131">
+        <v>1</v>
+      </c>
+      <c r="S131">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A132" s="16">
+        <v>332</v>
+      </c>
+      <c r="B132" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+      <c r="I132">
+        <v>1</v>
+      </c>
+      <c r="M132">
+        <v>1</v>
+      </c>
+      <c r="N132">
+        <v>1</v>
+      </c>
+      <c r="O132">
+        <v>1</v>
+      </c>
+      <c r="P132">
+        <v>1</v>
+      </c>
+      <c r="S132">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A133" s="16">
+        <v>333</v>
+      </c>
+      <c r="B133" s="1">
+        <v>2020</v>
+      </c>
+      <c r="J133">
+        <v>1</v>
+      </c>
+      <c r="S133">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A134" s="16">
+        <v>345</v>
+      </c>
+      <c r="B134" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H134">
+        <v>1</v>
+      </c>
+      <c r="N134">
+        <v>1</v>
+      </c>
+      <c r="S134">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A135" s="16">
+        <v>348</v>
+      </c>
+      <c r="B135" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H135">
+        <v>1</v>
+      </c>
+      <c r="S135">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A136" s="16">
+        <v>360</v>
+      </c>
+      <c r="B136" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H136">
+        <v>1</v>
+      </c>
+      <c r="J136">
+        <v>1</v>
+      </c>
+      <c r="R136">
+        <v>1</v>
+      </c>
+      <c r="S136">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A137" s="16">
+        <v>365</v>
+      </c>
+      <c r="B137" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H137">
+        <v>1</v>
+      </c>
+      <c r="J137">
+        <v>1</v>
+      </c>
+      <c r="S137">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A138" s="16">
+        <v>368</v>
+      </c>
+      <c r="B138" s="1">
+        <v>2021</v>
+      </c>
+      <c r="N138">
+        <v>1</v>
+      </c>
+      <c r="S138">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A139" s="16">
+        <v>374</v>
+      </c>
+      <c r="B139" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H139">
+        <v>1</v>
+      </c>
+      <c r="J139">
+        <v>1</v>
+      </c>
+      <c r="S139">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A140" s="16">
+        <v>375</v>
+      </c>
+      <c r="B140" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="N140">
+        <v>1</v>
+      </c>
+      <c r="S140">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A141" s="16">
+        <v>376</v>
+      </c>
+      <c r="B141" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H141">
+        <v>1</v>
+      </c>
+      <c r="J141">
+        <v>1</v>
+      </c>
+      <c r="S141">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A142" s="16">
+        <v>381</v>
+      </c>
+      <c r="B142" s="1">
+        <v>2020</v>
+      </c>
+      <c r="J142">
+        <v>1</v>
+      </c>
+      <c r="S142">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A143" s="16">
+        <v>385</v>
+      </c>
+      <c r="B143" s="1">
+        <v>2021</v>
+      </c>
+      <c r="O143">
+        <v>1</v>
+      </c>
+      <c r="S143">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A144" s="16">
+        <v>386</v>
+      </c>
+      <c r="B144" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H144">
+        <v>1</v>
+      </c>
+      <c r="N144">
+        <v>1</v>
+      </c>
+      <c r="S144">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A145" s="16">
+        <v>387</v>
+      </c>
+      <c r="B145" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H145">
+        <v>1</v>
+      </c>
+      <c r="J145">
+        <v>1</v>
+      </c>
+      <c r="S145">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A146" s="16">
+        <v>388</v>
+      </c>
+      <c r="B146" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="S146">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A147" s="16">
+        <v>392</v>
+      </c>
+      <c r="B147" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H147">
+        <v>1</v>
+      </c>
+      <c r="J147">
+        <v>1</v>
+      </c>
+      <c r="N147">
+        <v>1</v>
+      </c>
+      <c r="R147">
+        <v>1</v>
+      </c>
+      <c r="S147">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A148" s="16">
+        <v>394</v>
+      </c>
+      <c r="B148" s="1">
+        <v>2020</v>
+      </c>
+      <c r="H148">
+        <v>1</v>
+      </c>
+      <c r="N148">
+        <v>1</v>
+      </c>
+      <c r="O148">
+        <v>1</v>
+      </c>
+      <c r="S148">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A149" s="16">
+        <v>395</v>
+      </c>
+      <c r="B149" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H149">
+        <v>1</v>
+      </c>
+      <c r="J149">
+        <v>1</v>
+      </c>
+      <c r="N149">
+        <v>1</v>
+      </c>
+      <c r="P149">
+        <v>1</v>
+      </c>
+      <c r="Q149">
+        <v>1</v>
+      </c>
+      <c r="R149">
+        <v>1</v>
+      </c>
+      <c r="S149">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A150" s="16">
+        <v>402</v>
+      </c>
+      <c r="B150" s="1">
+        <v>2019</v>
+      </c>
+      <c r="J150">
+        <v>1</v>
+      </c>
+      <c r="R150">
+        <v>1</v>
+      </c>
+      <c r="S150">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A151" s="16">
+        <v>404</v>
+      </c>
+      <c r="B151" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H151">
+        <v>1</v>
+      </c>
+      <c r="J151">
+        <v>1</v>
+      </c>
+      <c r="N151">
+        <v>1</v>
+      </c>
+      <c r="O151">
+        <v>1</v>
+      </c>
+      <c r="S151">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A152" s="16">
+        <v>406</v>
+      </c>
+      <c r="B152" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H152">
+        <v>1</v>
+      </c>
+      <c r="S152">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A153" s="16">
+        <v>408</v>
+      </c>
+      <c r="B153" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+      <c r="H153">
+        <v>1</v>
+      </c>
+      <c r="J153">
+        <v>1</v>
+      </c>
+      <c r="S153">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A154" s="16">
+        <v>409</v>
+      </c>
+      <c r="B154" s="1">
+        <v>2019</v>
+      </c>
+      <c r="J154">
+        <v>1</v>
+      </c>
+      <c r="S154">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A155" s="16">
+        <v>410</v>
+      </c>
+      <c r="B155" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H155">
+        <v>1</v>
+      </c>
+      <c r="J155">
+        <v>1</v>
+      </c>
+      <c r="O155">
+        <v>1</v>
+      </c>
+      <c r="S155">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A156" s="16">
+        <v>411</v>
+      </c>
+      <c r="B156" s="1">
+        <v>2019</v>
+      </c>
+      <c r="J156">
+        <v>1</v>
+      </c>
+      <c r="R156">
+        <v>1</v>
+      </c>
+      <c r="S156">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A157" s="16">
+        <v>413</v>
+      </c>
+      <c r="B157" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H157">
+        <v>1</v>
+      </c>
+      <c r="J157">
+        <v>1</v>
+      </c>
+      <c r="S157">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A158" s="16">
+        <v>419</v>
+      </c>
+      <c r="B158" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H158">
+        <v>1</v>
+      </c>
+      <c r="S158">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A159" s="16">
+        <v>423</v>
+      </c>
+      <c r="B159" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H159">
+        <v>1</v>
+      </c>
+      <c r="S159">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A160" s="16">
+        <v>424</v>
+      </c>
+      <c r="B160" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H160">
+        <v>1</v>
+      </c>
+      <c r="J160">
+        <v>1</v>
+      </c>
+      <c r="S160">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A161" s="16">
+        <v>425</v>
+      </c>
+      <c r="B161" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H161">
+        <v>1</v>
+      </c>
+      <c r="J161">
+        <v>1</v>
+      </c>
+      <c r="S161">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A162" s="16">
+        <v>432</v>
+      </c>
+      <c r="B162" s="1">
+        <v>2019</v>
+      </c>
+      <c r="J162">
+        <v>1</v>
+      </c>
+      <c r="S162">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A163" s="16">
+        <v>436</v>
+      </c>
+      <c r="B163" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H163">
+        <v>1</v>
+      </c>
+      <c r="N163">
+        <v>1</v>
+      </c>
+      <c r="S163">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A164" s="16">
+        <v>438</v>
+      </c>
+      <c r="B164" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H164">
+        <v>1</v>
+      </c>
+      <c r="S164">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A165" s="16">
+        <v>440</v>
+      </c>
+      <c r="B165" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H165">
+        <v>1</v>
+      </c>
+      <c r="J165">
+        <v>1</v>
+      </c>
+      <c r="S165">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A166" s="16">
+        <v>441</v>
+      </c>
+      <c r="B166" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H166">
+        <v>1</v>
+      </c>
+      <c r="S166">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A167" s="16">
+        <v>442</v>
+      </c>
+      <c r="B167" s="1">
+        <v>2019</v>
+      </c>
+      <c r="J167">
+        <v>1</v>
+      </c>
+      <c r="S167">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A168" s="16">
+        <v>443</v>
+      </c>
+      <c r="B168" s="1">
+        <v>2019</v>
+      </c>
+      <c r="O168">
+        <v>1</v>
+      </c>
+      <c r="S168">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A169" s="16">
+        <v>447</v>
+      </c>
+      <c r="B169" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H169">
+        <v>1</v>
+      </c>
+      <c r="N169">
+        <v>1</v>
+      </c>
+      <c r="S169">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A170" s="16">
+        <v>451</v>
+      </c>
+      <c r="B170" s="1">
+        <v>2019</v>
+      </c>
+      <c r="J170">
+        <v>1</v>
+      </c>
+      <c r="S170">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A171" s="16">
+        <v>452</v>
+      </c>
+      <c r="B171" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H171">
+        <v>1</v>
+      </c>
+      <c r="S171">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A172" s="16">
+        <v>455</v>
+      </c>
+      <c r="B172" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H172">
+        <v>1</v>
+      </c>
+      <c r="S172">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A173" s="16">
+        <v>456</v>
+      </c>
+      <c r="B173" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H173">
+        <v>1</v>
+      </c>
+      <c r="S173">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A174" s="17"/>
+      <c r="B174" s="17"/>
+      <c r="C174" s="17">
+        <v>1</v>
+      </c>
+      <c r="D174" s="17">
+        <v>11</v>
+      </c>
+      <c r="E174" s="17">
+        <v>4</v>
+      </c>
+      <c r="F174" s="17"/>
+      <c r="G174" s="17">
+        <v>3</v>
+      </c>
+      <c r="H174" s="17">
+        <v>112</v>
+      </c>
+      <c r="I174" s="17">
+        <v>1</v>
+      </c>
+      <c r="J174" s="17">
+        <v>96</v>
+      </c>
+      <c r="K174" s="17">
+        <v>1</v>
+      </c>
+      <c r="L174" s="17"/>
+      <c r="M174" s="17">
+        <v>3</v>
+      </c>
+      <c r="N174" s="17">
+        <v>38</v>
+      </c>
+      <c r="O174" s="17">
+        <v>18</v>
+      </c>
+      <c r="P174" s="17">
+        <v>10</v>
+      </c>
+      <c r="Q174" s="17">
+        <v>9</v>
+      </c>
+      <c r="R174" s="17">
+        <v>29</v>
+      </c>
+      <c r="S174" s="18">
+        <f>SUM(Table1[[#This Row],[ Asociación]:[ Regresión]])</f>
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC07773-676A-4489-9C35-33E143940D9C}">
   <dimension ref="A1:E38"/>
   <sheetViews>

</xml_diff>